<commit_message>
Carga de excel inventario (falta)
Por favor realizar composer update
</commit_message>
<xml_diff>
--- a/public/assets-Internas/smartbar.xlsx
+++ b/public/assets-Internas/smartbar.xlsx
@@ -13,14 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Inventario" sheetId="1" r:id="rId1"/>
-    <sheet name="Proveedores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -406,7 +405,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -885,40 +884,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Proveedores!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>